<commit_message>
Update ca_app with latest admin access form, requirements, and UI fixes
</commit_message>
<xml_diff>
--- a/data/Properties_geocoded.xlsx
+++ b/data/Properties_geocoded.xlsx
@@ -1,26 +1,39 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29127"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29231"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/b3db30460c098f93/Desktop/--New folder for app/data/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://chamberlinass-my.sharepoint.com/personal/adrian_ca-mgmt_com/Documents/Desktop/Code Projects/New Map app/ca_app-main/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="48" documentId="11_242171AAD3B0D16F8B193711595ED87656CCE5E3" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{75CE8D79-093F-48EB-BEDE-EECF7755B044}"/>
+  <xr:revisionPtr revIDLastSave="61" documentId="11_242171AAD3B0D16F8B193711595ED87656CCE5E3" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{476212F5-9E62-47F8-A73A-6E60B26985A9}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21120" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="0"/>
+  <calcPr calcId="191029"/>
+  <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="583" uniqueCount="253">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="576" uniqueCount="251">
   <si>
     <t>PropertyID</t>
   </si>
@@ -421,9 +434,6 @@
     <t>Mountain Valley Apartments</t>
   </si>
   <si>
-    <t>12 W Dobbins Rd</t>
-  </si>
-  <si>
     <t>John</t>
   </si>
   <si>
@@ -484,27 +494,18 @@
     <t>Revival Midtown Apartments</t>
   </si>
   <si>
-    <t>711 W Indian School Rd</t>
-  </si>
-  <si>
     <t>Denise</t>
   </si>
   <si>
     <t>Riviera Park Apartments</t>
   </si>
   <si>
-    <t>1810 E Bell Rd</t>
-  </si>
-  <si>
     <t>Sahara Palms &amp; Playa Apartments</t>
   </si>
   <si>
     <t>4325 N 23rd Ave</t>
   </si>
   <si>
-    <t>San Augustine Apartments</t>
-  </si>
-  <si>
     <t>2047 W Hayward Ave</t>
   </si>
   <si>
@@ -679,15 +680,6 @@
     <t>Amy &amp; Ed</t>
   </si>
   <si>
-    <t>Urban 148 Apartments</t>
-  </si>
-  <si>
-    <t>1609 W Glendale Ave</t>
-  </si>
-  <si>
-    <t>Maxx</t>
-  </si>
-  <si>
     <t>The Valencia Townhomes</t>
   </si>
   <si>
@@ -779,6 +771,21 @@
   </si>
   <si>
     <t>Robert Alvarado</t>
+  </si>
+  <si>
+    <t>120 W Dobbins Rd</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1220 E Medlock Dr. </t>
+  </si>
+  <si>
+    <t>125 S Dobson Rd</t>
+  </si>
+  <si>
+    <t>2300 W San Angelo St</t>
+  </si>
+  <si>
+    <t>San Augustine Townhomes</t>
   </si>
 </sst>
 </file>
@@ -1143,39 +1150,39 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:P83"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A40" workbookViewId="0">
-      <selection sqref="A1:L1048576"/>
+    <sheetView tabSelected="1" topLeftCell="A69" workbookViewId="0">
+      <selection activeCell="B77" sqref="B77:L77"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="10.5703125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="32.28515625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="24.42578125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="12.7109375" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="5.5703125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="10.54296875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="32.26953125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="24.453125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="12.7265625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="5.54296875" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="6" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="10.5703125" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="17.28515625" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="31.42578125" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="35.140625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="10.54296875" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="17.26953125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="31.453125" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="35.1796875" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="12" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="12.7109375" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="103.42578125" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="15.7109375" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="14.5703125" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="19.85546875" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="12.7265625" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="103.453125" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="15.7265625" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="14.54296875" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="19.81640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>235</v>
+        <v>228</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>236</v>
+        <v>229</v>
       </c>
       <c r="D1" s="1" t="s">
         <v>1</v>
@@ -1209,7 +1216,7 @@
       <c r="O1" s="1"/>
       <c r="P1" s="1"/>
     </row>
-    <row r="2" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A2">
         <v>1</v>
       </c>
@@ -1232,10 +1239,10 @@
         <v>90</v>
       </c>
       <c r="H2" t="s">
-        <v>247</v>
+        <v>240</v>
       </c>
       <c r="I2" t="s">
-        <v>250</v>
+        <v>243</v>
       </c>
       <c r="J2" t="s">
         <v>14</v>
@@ -1247,7 +1254,7 @@
         <v>-112.028401</v>
       </c>
     </row>
-    <row r="3" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A3">
         <v>2</v>
       </c>
@@ -1270,10 +1277,10 @@
         <v>104</v>
       </c>
       <c r="H3" t="s">
-        <v>244</v>
+        <v>237</v>
       </c>
       <c r="I3" t="s">
-        <v>252</v>
+        <v>245</v>
       </c>
       <c r="J3" t="s">
         <v>18</v>
@@ -1285,7 +1292,7 @@
         <v>-112.0119</v>
       </c>
     </row>
-    <row r="4" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A4">
         <v>3</v>
       </c>
@@ -1308,10 +1315,10 @@
         <v>258</v>
       </c>
       <c r="H4" t="s">
-        <v>243</v>
+        <v>236</v>
       </c>
       <c r="I4" t="s">
-        <v>248</v>
+        <v>241</v>
       </c>
       <c r="J4" t="s">
         <v>21</v>
@@ -1323,7 +1330,7 @@
         <v>-111.9918</v>
       </c>
     </row>
-    <row r="5" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A5">
         <v>4</v>
       </c>
@@ -1346,10 +1353,10 @@
         <v>117</v>
       </c>
       <c r="H5" t="s">
-        <v>245</v>
+        <v>238</v>
       </c>
       <c r="I5" t="s">
-        <v>248</v>
+        <v>241</v>
       </c>
       <c r="J5" t="s">
         <v>24</v>
@@ -1361,7 +1368,7 @@
         <v>-112.072844</v>
       </c>
     </row>
-    <row r="6" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A6">
         <v>5</v>
       </c>
@@ -1384,10 +1391,10 @@
         <v>165</v>
       </c>
       <c r="H6" t="s">
+        <v>238</v>
+      </c>
+      <c r="I6" t="s">
         <v>245</v>
-      </c>
-      <c r="I6" t="s">
-        <v>252</v>
       </c>
       <c r="J6" t="s">
         <v>28</v>
@@ -1399,7 +1406,7 @@
         <v>-111.8920811</v>
       </c>
     </row>
-    <row r="7" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A7">
         <v>6</v>
       </c>
@@ -1422,10 +1429,10 @@
         <v>142</v>
       </c>
       <c r="H7" t="s">
-        <v>238</v>
+        <v>231</v>
       </c>
       <c r="I7" t="s">
-        <v>250</v>
+        <v>243</v>
       </c>
       <c r="J7" t="s">
         <v>31</v>
@@ -1437,7 +1444,7 @@
         <v>-112.0164541</v>
       </c>
     </row>
-    <row r="8" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A8">
         <v>7</v>
       </c>
@@ -1460,10 +1467,10 @@
         <v>148</v>
       </c>
       <c r="H8" t="s">
-        <v>243</v>
+        <v>236</v>
       </c>
       <c r="I8" t="s">
-        <v>248</v>
+        <v>241</v>
       </c>
       <c r="J8" t="s">
         <v>21</v>
@@ -1475,7 +1482,7 @@
         <v>-111.9871246</v>
       </c>
     </row>
-    <row r="9" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A9">
         <v>8</v>
       </c>
@@ -1498,10 +1505,10 @@
         <v>88</v>
       </c>
       <c r="H9" t="s">
-        <v>240</v>
+        <v>233</v>
       </c>
       <c r="I9" t="s">
-        <v>249</v>
+        <v>242</v>
       </c>
       <c r="J9" t="s">
         <v>37</v>
@@ -1513,7 +1520,7 @@
         <v>-111.6641503</v>
       </c>
     </row>
-    <row r="10" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A10">
         <v>9</v>
       </c>
@@ -1536,10 +1543,10 @@
         <v>160</v>
       </c>
       <c r="H10" t="s">
-        <v>244</v>
+        <v>237</v>
       </c>
       <c r="I10" t="s">
-        <v>252</v>
+        <v>245</v>
       </c>
       <c r="J10" t="s">
         <v>40</v>
@@ -1551,7 +1558,7 @@
         <v>-112.0971</v>
       </c>
     </row>
-    <row r="11" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A11">
         <v>10</v>
       </c>
@@ -1574,10 +1581,10 @@
         <v>285</v>
       </c>
       <c r="H11" t="s">
-        <v>240</v>
+        <v>233</v>
       </c>
       <c r="I11" t="s">
-        <v>249</v>
+        <v>242</v>
       </c>
       <c r="J11" t="s">
         <v>44</v>
@@ -1589,7 +1596,7 @@
         <v>-111.8815163</v>
       </c>
     </row>
-    <row r="12" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A12">
         <v>11</v>
       </c>
@@ -1612,10 +1619,10 @@
         <v>175</v>
       </c>
       <c r="H12" t="s">
-        <v>240</v>
+        <v>233</v>
       </c>
       <c r="I12" t="s">
-        <v>250</v>
+        <v>243</v>
       </c>
       <c r="J12" t="s">
         <v>31</v>
@@ -1627,7 +1634,7 @@
         <v>-112.0583381</v>
       </c>
     </row>
-    <row r="13" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A13">
         <v>12</v>
       </c>
@@ -1650,10 +1657,10 @@
         <v>42</v>
       </c>
       <c r="H13" t="s">
-        <v>246</v>
+        <v>239</v>
       </c>
       <c r="I13" t="s">
-        <v>252</v>
+        <v>245</v>
       </c>
       <c r="J13" t="s">
         <v>49</v>
@@ -1665,7 +1672,7 @@
         <v>-111.9838785</v>
       </c>
     </row>
-    <row r="14" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A14">
         <v>13</v>
       </c>
@@ -1688,10 +1695,10 @@
         <v>9</v>
       </c>
       <c r="H14" t="s">
-        <v>244</v>
+        <v>237</v>
       </c>
       <c r="I14" t="s">
-        <v>252</v>
+        <v>245</v>
       </c>
       <c r="J14" t="s">
         <v>18</v>
@@ -1703,7 +1710,7 @@
         <v>-111.9350725</v>
       </c>
     </row>
-    <row r="15" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A15">
         <v>14</v>
       </c>
@@ -1726,10 +1733,10 @@
         <v>256</v>
       </c>
       <c r="H15" t="s">
-        <v>247</v>
+        <v>240</v>
       </c>
       <c r="I15" t="s">
-        <v>252</v>
+        <v>245</v>
       </c>
       <c r="J15" t="s">
         <v>55</v>
@@ -1741,7 +1748,7 @@
         <v>-112.1543454</v>
       </c>
     </row>
-    <row r="16" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A16">
         <v>15</v>
       </c>
@@ -1764,10 +1771,10 @@
         <v>64</v>
       </c>
       <c r="H16" t="s">
+        <v>238</v>
+      </c>
+      <c r="I16" t="s">
         <v>245</v>
-      </c>
-      <c r="I16" t="s">
-        <v>252</v>
       </c>
       <c r="J16" t="s">
         <v>58</v>
@@ -1779,7 +1786,7 @@
         <v>-112.1126534</v>
       </c>
     </row>
-    <row r="17" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A17">
         <v>16</v>
       </c>
@@ -1802,10 +1809,10 @@
         <v>156</v>
       </c>
       <c r="H17" t="s">
-        <v>240</v>
+        <v>233</v>
       </c>
       <c r="I17" t="s">
-        <v>249</v>
+        <v>242</v>
       </c>
       <c r="J17" t="s">
         <v>62</v>
@@ -1817,7 +1824,7 @@
         <v>-111.8444016</v>
       </c>
     </row>
-    <row r="18" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A18">
         <v>17</v>
       </c>
@@ -1840,10 +1847,10 @@
         <v>128</v>
       </c>
       <c r="H18" t="s">
-        <v>239</v>
+        <v>232</v>
       </c>
       <c r="I18" t="s">
-        <v>251</v>
+        <v>244</v>
       </c>
       <c r="J18" t="s">
         <v>66</v>
@@ -1855,7 +1862,7 @@
         <v>-110.84705409999999</v>
       </c>
     </row>
-    <row r="19" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A19">
         <v>18</v>
       </c>
@@ -1878,10 +1885,10 @@
         <v>198</v>
       </c>
       <c r="H19" t="s">
-        <v>240</v>
+        <v>233</v>
       </c>
       <c r="I19" t="s">
-        <v>252</v>
+        <v>245</v>
       </c>
       <c r="J19" t="s">
         <v>69</v>
@@ -1893,7 +1900,7 @@
         <v>-112.0830137</v>
       </c>
     </row>
-    <row r="20" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A20">
         <v>19</v>
       </c>
@@ -1916,10 +1923,10 @@
         <v>75</v>
       </c>
       <c r="H20" t="s">
-        <v>244</v>
+        <v>237</v>
       </c>
       <c r="I20" t="s">
-        <v>248</v>
+        <v>241</v>
       </c>
       <c r="J20" t="s">
         <v>72</v>
@@ -1931,7 +1938,7 @@
         <v>-112.00530000000001</v>
       </c>
     </row>
-    <row r="21" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A21">
         <v>20</v>
       </c>
@@ -1954,10 +1961,10 @@
         <v>112</v>
       </c>
       <c r="H21" t="s">
-        <v>239</v>
+        <v>232</v>
       </c>
       <c r="I21" t="s">
-        <v>251</v>
+        <v>244</v>
       </c>
       <c r="J21" t="s">
         <v>76</v>
@@ -1969,7 +1976,7 @@
         <v>-110.2912384</v>
       </c>
     </row>
-    <row r="22" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A22">
         <v>21</v>
       </c>
@@ -1992,10 +1999,10 @@
         <v>144</v>
       </c>
       <c r="H22" t="s">
+        <v>238</v>
+      </c>
+      <c r="I22" t="s">
         <v>245</v>
-      </c>
-      <c r="I22" t="s">
-        <v>252</v>
       </c>
       <c r="J22" t="s">
         <v>58</v>
@@ -2007,7 +2014,7 @@
         <v>-112.0481087</v>
       </c>
     </row>
-    <row r="23" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A23">
         <v>22</v>
       </c>
@@ -2030,10 +2037,10 @@
         <v>152</v>
       </c>
       <c r="H23" t="s">
-        <v>239</v>
+        <v>232</v>
       </c>
       <c r="I23" t="s">
-        <v>251</v>
+        <v>244</v>
       </c>
       <c r="J23" t="s">
         <v>76</v>
@@ -2045,7 +2052,7 @@
         <v>-110.297515</v>
       </c>
     </row>
-    <row r="24" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A24">
         <v>23</v>
       </c>
@@ -2068,10 +2075,10 @@
         <v>265</v>
       </c>
       <c r="H24" t="s">
+        <v>236</v>
+      </c>
+      <c r="I24" t="s">
         <v>243</v>
-      </c>
-      <c r="I24" t="s">
-        <v>250</v>
       </c>
       <c r="J24" t="s">
         <v>83</v>
@@ -2083,7 +2090,7 @@
         <v>-112.10113149999999</v>
       </c>
     </row>
-    <row r="25" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A25">
         <v>24</v>
       </c>
@@ -2106,10 +2113,10 @@
         <v>164</v>
       </c>
       <c r="H25" t="s">
-        <v>243</v>
+        <v>236</v>
       </c>
       <c r="I25" t="s">
-        <v>248</v>
+        <v>241</v>
       </c>
       <c r="J25" t="s">
         <v>21</v>
@@ -2121,7 +2128,7 @@
         <v>-111.78984699999999</v>
       </c>
     </row>
-    <row r="26" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A26">
         <v>25</v>
       </c>
@@ -2144,10 +2151,10 @@
         <v>208</v>
       </c>
       <c r="H26" t="s">
-        <v>238</v>
+        <v>231</v>
       </c>
       <c r="I26" t="s">
-        <v>250</v>
+        <v>243</v>
       </c>
       <c r="J26" t="s">
         <v>89</v>
@@ -2159,7 +2166,7 @@
         <v>-112.133557</v>
       </c>
     </row>
-    <row r="27" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A27">
         <v>26</v>
       </c>
@@ -2182,10 +2189,10 @@
         <v>150</v>
       </c>
       <c r="H27" t="s">
-        <v>240</v>
+        <v>233</v>
       </c>
       <c r="I27" t="s">
-        <v>249</v>
+        <v>242</v>
       </c>
       <c r="J27" t="s">
         <v>92</v>
@@ -2197,7 +2204,7 @@
         <v>-112.1021367</v>
       </c>
     </row>
-    <row r="28" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A28">
         <v>27</v>
       </c>
@@ -2220,10 +2227,10 @@
         <v>108</v>
       </c>
       <c r="H28" t="s">
-        <v>245</v>
+        <v>238</v>
       </c>
       <c r="I28" t="s">
-        <v>250</v>
+        <v>243</v>
       </c>
       <c r="J28" t="s">
         <v>95</v>
@@ -2235,7 +2242,7 @@
         <v>-112.0402059</v>
       </c>
     </row>
-    <row r="29" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A29">
         <v>28</v>
       </c>
@@ -2258,7 +2265,7 @@
         <v>120</v>
       </c>
       <c r="H29" t="s">
-        <v>238</v>
+        <v>231</v>
       </c>
       <c r="J29" t="s">
         <v>100</v>
@@ -2267,10 +2274,10 @@
         <v>30.019852199999999</v>
       </c>
       <c r="L29" t="s">
-        <v>237</v>
-      </c>
-    </row>
-    <row r="30" spans="1:12" x14ac:dyDescent="0.25">
+        <v>230</v>
+      </c>
+    </row>
+    <row r="30" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A30">
         <v>29</v>
       </c>
@@ -2293,10 +2300,10 @@
         <v>37</v>
       </c>
       <c r="H30" t="s">
+        <v>238</v>
+      </c>
+      <c r="I30" t="s">
         <v>245</v>
-      </c>
-      <c r="I30" t="s">
-        <v>252</v>
       </c>
       <c r="J30" t="s">
         <v>58</v>
@@ -2308,7 +2315,7 @@
         <v>-112.0704107</v>
       </c>
     </row>
-    <row r="31" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A31">
         <v>30</v>
       </c>
@@ -2331,10 +2338,10 @@
         <v>36</v>
       </c>
       <c r="H31" t="s">
+        <v>238</v>
+      </c>
+      <c r="I31" t="s">
         <v>245</v>
-      </c>
-      <c r="I31" t="s">
-        <v>252</v>
       </c>
       <c r="J31" t="s">
         <v>58</v>
@@ -2346,7 +2353,7 @@
         <v>-112.0706807</v>
       </c>
     </row>
-    <row r="32" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A32">
         <v>31</v>
       </c>
@@ -2369,10 +2376,10 @@
         <v>87</v>
       </c>
       <c r="H32" t="s">
-        <v>247</v>
+        <v>240</v>
       </c>
       <c r="I32" t="s">
-        <v>250</v>
+        <v>243</v>
       </c>
       <c r="J32" t="s">
         <v>107</v>
@@ -2384,7 +2391,7 @@
         <v>-112.0652674</v>
       </c>
     </row>
-    <row r="33" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A33">
         <v>32</v>
       </c>
@@ -2407,10 +2414,10 @@
         <v>154</v>
       </c>
       <c r="H33" t="s">
-        <v>240</v>
+        <v>233</v>
       </c>
       <c r="I33" t="s">
-        <v>249</v>
+        <v>242</v>
       </c>
       <c r="J33" t="s">
         <v>62</v>
@@ -2422,7 +2429,7 @@
         <v>-111.93797309999999</v>
       </c>
     </row>
-    <row r="34" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A34">
         <v>33</v>
       </c>
@@ -2445,10 +2452,10 @@
         <v>163</v>
       </c>
       <c r="H34" t="s">
-        <v>243</v>
+        <v>236</v>
       </c>
       <c r="I34" t="s">
-        <v>248</v>
+        <v>241</v>
       </c>
       <c r="J34" t="s">
         <v>21</v>
@@ -2460,7 +2467,7 @@
         <v>-111.8588345</v>
       </c>
     </row>
-    <row r="35" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A35">
         <v>34</v>
       </c>
@@ -2483,10 +2490,10 @@
         <v>120</v>
       </c>
       <c r="H35" t="s">
-        <v>242</v>
+        <v>235</v>
       </c>
       <c r="I35" t="s">
-        <v>251</v>
+        <v>244</v>
       </c>
       <c r="J35" t="s">
         <v>116</v>
@@ -2498,7 +2505,7 @@
         <v>-106.5784922</v>
       </c>
     </row>
-    <row r="36" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A36">
         <v>35</v>
       </c>
@@ -2521,10 +2528,10 @@
         <v>24</v>
       </c>
       <c r="H36" t="s">
-        <v>240</v>
+        <v>233</v>
       </c>
       <c r="I36" t="s">
-        <v>249</v>
+        <v>242</v>
       </c>
       <c r="J36" t="s">
         <v>119</v>
@@ -2536,7 +2543,7 @@
         <v>-111.909007</v>
       </c>
     </row>
-    <row r="37" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A37">
         <v>36</v>
       </c>
@@ -2559,10 +2566,10 @@
         <v>301</v>
       </c>
       <c r="H37" t="s">
-        <v>247</v>
+        <v>240</v>
       </c>
       <c r="I37" t="s">
-        <v>250</v>
+        <v>243</v>
       </c>
       <c r="J37" t="s">
         <v>122</v>
@@ -2574,7 +2581,7 @@
         <v>-112.1788092</v>
       </c>
     </row>
-    <row r="38" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A38">
         <v>37</v>
       </c>
@@ -2597,10 +2604,10 @@
         <v>82</v>
       </c>
       <c r="H38" t="s">
-        <v>245</v>
+        <v>238</v>
       </c>
       <c r="I38" t="s">
-        <v>248</v>
+        <v>241</v>
       </c>
       <c r="J38" t="s">
         <v>125</v>
@@ -2612,7 +2619,7 @@
         <v>-111.67333000000001</v>
       </c>
     </row>
-    <row r="39" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A39">
         <v>38</v>
       </c>
@@ -2635,10 +2642,10 @@
         <v>50</v>
       </c>
       <c r="H39" t="s">
-        <v>247</v>
+        <v>240</v>
       </c>
       <c r="I39" t="s">
-        <v>250</v>
+        <v>243</v>
       </c>
       <c r="J39" t="s">
         <v>129</v>
@@ -2650,7 +2657,7 @@
         <v>-112.15970040000001</v>
       </c>
     </row>
-    <row r="40" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A40">
         <v>39</v>
       </c>
@@ -2673,10 +2680,10 @@
         <v>228</v>
       </c>
       <c r="H40" t="s">
-        <v>239</v>
+        <v>232</v>
       </c>
       <c r="I40" t="s">
-        <v>251</v>
+        <v>244</v>
       </c>
       <c r="J40" t="s">
         <v>76</v>
@@ -2688,7 +2695,7 @@
         <v>-110.253815</v>
       </c>
     </row>
-    <row r="41" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A41">
         <v>40</v>
       </c>
@@ -2696,7 +2703,7 @@
         <v>132</v>
       </c>
       <c r="C41" t="s">
-        <v>133</v>
+        <v>246</v>
       </c>
       <c r="D41" t="s">
         <v>12</v>
@@ -2711,13 +2718,13 @@
         <v>45</v>
       </c>
       <c r="H41" t="s">
-        <v>245</v>
+        <v>238</v>
       </c>
       <c r="I41" t="s">
-        <v>248</v>
+        <v>241</v>
       </c>
       <c r="J41" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="K41">
         <v>33.363639499999998</v>
@@ -2726,18 +2733,18 @@
         <v>-112.07502909999999</v>
       </c>
     </row>
-    <row r="42" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A42">
         <v>41</v>
       </c>
       <c r="B42" t="s">
+        <v>134</v>
+      </c>
+      <c r="C42" t="s">
         <v>135</v>
       </c>
-      <c r="C42" t="s">
+      <c r="D42" t="s">
         <v>136</v>
-      </c>
-      <c r="D42" t="s">
-        <v>137</v>
       </c>
       <c r="E42" t="s">
         <v>13</v>
@@ -2749,13 +2756,13 @@
         <v>100</v>
       </c>
       <c r="H42" t="s">
-        <v>247</v>
+        <v>240</v>
       </c>
       <c r="I42" t="s">
-        <v>252</v>
+        <v>245</v>
       </c>
       <c r="J42" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="K42">
         <v>33.59019</v>
@@ -2764,15 +2771,15 @@
         <v>-112.22041</v>
       </c>
     </row>
-    <row r="43" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A43">
         <v>42</v>
       </c>
       <c r="B43" t="s">
+        <v>138</v>
+      </c>
+      <c r="C43" t="s">
         <v>139</v>
-      </c>
-      <c r="C43" t="s">
-        <v>140</v>
       </c>
       <c r="D43" t="s">
         <v>27</v>
@@ -2787,10 +2794,10 @@
         <v>244</v>
       </c>
       <c r="H43" t="s">
-        <v>246</v>
+        <v>239</v>
       </c>
       <c r="I43" t="s">
-        <v>252</v>
+        <v>245</v>
       </c>
       <c r="J43" t="s">
         <v>76</v>
@@ -2802,15 +2809,15 @@
         <v>-111.923278</v>
       </c>
     </row>
-    <row r="44" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A44">
         <v>43</v>
       </c>
       <c r="B44" t="s">
+        <v>140</v>
+      </c>
+      <c r="C44" t="s">
         <v>141</v>
-      </c>
-      <c r="C44" t="s">
-        <v>142</v>
       </c>
       <c r="D44" t="s">
         <v>12</v>
@@ -2825,13 +2832,13 @@
         <v>220</v>
       </c>
       <c r="H44" t="s">
-        <v>240</v>
+        <v>233</v>
       </c>
       <c r="I44" t="s">
-        <v>249</v>
+        <v>242</v>
       </c>
       <c r="J44" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="K44">
         <v>33.529920699999998</v>
@@ -2840,15 +2847,15 @@
         <v>-112.06444329999999</v>
       </c>
     </row>
-    <row r="45" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A45">
         <v>44</v>
       </c>
       <c r="B45" t="s">
+        <v>143</v>
+      </c>
+      <c r="C45" t="s">
         <v>144</v>
-      </c>
-      <c r="C45" t="s">
-        <v>145</v>
       </c>
       <c r="D45" t="s">
         <v>12</v>
@@ -2863,13 +2870,13 @@
         <v>280</v>
       </c>
       <c r="H45" t="s">
-        <v>240</v>
+        <v>233</v>
       </c>
       <c r="I45" t="s">
-        <v>249</v>
+        <v>242</v>
       </c>
       <c r="J45" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="K45">
         <v>33.509409099999999</v>
@@ -2878,15 +2885,15 @@
         <v>-112.0803222</v>
       </c>
     </row>
-    <row r="46" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A46">
         <v>45</v>
       </c>
       <c r="B46" t="s">
+        <v>145</v>
+      </c>
+      <c r="C46" t="s">
         <v>146</v>
-      </c>
-      <c r="C46" t="s">
-        <v>147</v>
       </c>
       <c r="D46" t="s">
         <v>12</v>
@@ -2901,10 +2908,10 @@
         <v>214</v>
       </c>
       <c r="H46" t="s">
-        <v>240</v>
+        <v>233</v>
       </c>
       <c r="I46" t="s">
-        <v>249</v>
+        <v>242</v>
       </c>
       <c r="J46" t="s">
         <v>24</v>
@@ -2916,15 +2923,15 @@
         <v>-112.1117</v>
       </c>
     </row>
-    <row r="47" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A47">
         <v>46</v>
       </c>
       <c r="B47" t="s">
+        <v>147</v>
+      </c>
+      <c r="C47" t="s">
         <v>148</v>
-      </c>
-      <c r="C47" t="s">
-        <v>149</v>
       </c>
       <c r="D47" t="s">
         <v>12</v>
@@ -2939,13 +2946,13 @@
         <v>162</v>
       </c>
       <c r="H47" t="s">
-        <v>247</v>
+        <v>240</v>
       </c>
       <c r="I47" t="s">
-        <v>250</v>
+        <v>243</v>
       </c>
       <c r="J47" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="K47">
         <v>33.559951300000002</v>
@@ -2954,15 +2961,15 @@
         <v>-112.1167032</v>
       </c>
     </row>
-    <row r="48" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A48">
         <v>47</v>
       </c>
       <c r="B48" t="s">
+        <v>150</v>
+      </c>
+      <c r="C48" t="s">
         <v>151</v>
-      </c>
-      <c r="C48" t="s">
-        <v>152</v>
       </c>
       <c r="D48" t="s">
         <v>12</v>
@@ -2977,10 +2984,10 @@
         <v>26</v>
       </c>
       <c r="H48" t="s">
-        <v>245</v>
+        <v>238</v>
       </c>
       <c r="I48" t="s">
-        <v>250</v>
+        <v>243</v>
       </c>
       <c r="J48" t="s">
         <v>95</v>
@@ -2992,15 +2999,15 @@
         <v>-112.08121920000001</v>
       </c>
     </row>
-    <row r="49" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A49">
         <v>48</v>
       </c>
       <c r="B49" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="C49" t="s">
-        <v>154</v>
+        <v>247</v>
       </c>
       <c r="D49" t="s">
         <v>12</v>
@@ -3009,74 +3016,62 @@
         <v>13</v>
       </c>
       <c r="F49">
-        <v>85013</v>
+        <v>85014</v>
       </c>
       <c r="G49">
         <v>35</v>
       </c>
       <c r="H49" t="s">
-        <v>244</v>
+        <v>237</v>
       </c>
       <c r="I49" t="s">
-        <v>248</v>
+        <v>241</v>
       </c>
       <c r="J49" t="s">
-        <v>155</v>
-      </c>
-      <c r="K49">
-        <v>33.511504831575863</v>
-      </c>
-      <c r="L49">
-        <v>-112.055683</v>
-      </c>
-    </row>
-    <row r="50" spans="1:12" x14ac:dyDescent="0.25">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="50" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A50">
         <v>49</v>
       </c>
       <c r="B50" t="s">
-        <v>156</v>
+        <v>154</v>
       </c>
       <c r="C50" t="s">
-        <v>157</v>
+        <v>248</v>
       </c>
       <c r="D50" t="s">
-        <v>12</v>
+        <v>61</v>
       </c>
       <c r="E50" t="s">
         <v>13</v>
       </c>
       <c r="F50">
-        <v>85022</v>
+        <v>85224</v>
       </c>
       <c r="G50">
         <v>201</v>
       </c>
       <c r="H50" t="s">
-        <v>243</v>
+        <v>236</v>
       </c>
       <c r="I50" t="s">
-        <v>248</v>
+        <v>241</v>
       </c>
       <c r="J50" t="s">
         <v>21</v>
       </c>
-      <c r="K50">
-        <v>33.640509199999997</v>
-      </c>
-      <c r="L50">
-        <v>-112.04362519999999</v>
-      </c>
-    </row>
-    <row r="51" spans="1:12" x14ac:dyDescent="0.25">
+    </row>
+    <row r="51" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A51">
         <v>50</v>
       </c>
       <c r="B51" t="s">
-        <v>158</v>
+        <v>155</v>
       </c>
       <c r="C51" t="s">
-        <v>159</v>
+        <v>249</v>
       </c>
       <c r="D51" t="s">
         <v>12</v>
@@ -3085,36 +3080,30 @@
         <v>13</v>
       </c>
       <c r="F51">
-        <v>85015</v>
+        <v>85233</v>
       </c>
       <c r="G51">
         <v>840</v>
       </c>
       <c r="H51" t="s">
-        <v>243</v>
+        <v>236</v>
       </c>
       <c r="I51" t="s">
-        <v>248</v>
+        <v>241</v>
       </c>
       <c r="J51" t="s">
         <v>21</v>
       </c>
-      <c r="K51">
-        <v>33.368743000000002</v>
-      </c>
-      <c r="L51">
-        <v>-111.839252</v>
-      </c>
-    </row>
-    <row r="52" spans="1:12" x14ac:dyDescent="0.25">
+    </row>
+    <row r="52" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A52">
         <v>51</v>
       </c>
       <c r="B52" t="s">
-        <v>160</v>
+        <v>250</v>
       </c>
       <c r="C52" t="s">
-        <v>161</v>
+        <v>157</v>
       </c>
       <c r="D52" t="s">
         <v>12</v>
@@ -3129,13 +3118,13 @@
         <v>20</v>
       </c>
       <c r="H52" t="s">
-        <v>247</v>
+        <v>240</v>
       </c>
       <c r="I52" t="s">
-        <v>250</v>
+        <v>243</v>
       </c>
       <c r="J52" t="s">
-        <v>162</v>
+        <v>158</v>
       </c>
       <c r="K52">
         <v>33.550420000000003</v>
@@ -3144,15 +3133,15 @@
         <v>-112.103358</v>
       </c>
     </row>
-    <row r="53" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A53">
         <v>52</v>
       </c>
       <c r="B53" t="s">
-        <v>163</v>
+        <v>159</v>
       </c>
       <c r="C53" t="s">
-        <v>164</v>
+        <v>160</v>
       </c>
       <c r="D53" t="s">
         <v>12</v>
@@ -3167,10 +3156,10 @@
         <v>70</v>
       </c>
       <c r="H53" t="s">
+        <v>238</v>
+      </c>
+      <c r="I53" t="s">
         <v>245</v>
-      </c>
-      <c r="I53" t="s">
-        <v>252</v>
       </c>
       <c r="J53" t="s">
         <v>58</v>
@@ -3182,18 +3171,18 @@
         <v>-112.1176956</v>
       </c>
     </row>
-    <row r="54" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A54">
         <v>53</v>
       </c>
       <c r="B54" t="s">
-        <v>165</v>
+        <v>161</v>
       </c>
       <c r="C54" t="s">
-        <v>166</v>
+        <v>162</v>
       </c>
       <c r="D54" t="s">
-        <v>167</v>
+        <v>163</v>
       </c>
       <c r="E54" t="s">
         <v>99</v>
@@ -3205,7 +3194,7 @@
         <v>209</v>
       </c>
       <c r="H54" t="s">
-        <v>238</v>
+        <v>231</v>
       </c>
       <c r="J54" t="s">
         <v>100</v>
@@ -3217,15 +3206,15 @@
         <v>-95.554195399999998</v>
       </c>
     </row>
-    <row r="55" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A55">
         <v>54</v>
       </c>
       <c r="B55" t="s">
-        <v>168</v>
+        <v>164</v>
       </c>
       <c r="C55" t="s">
-        <v>169</v>
+        <v>165</v>
       </c>
       <c r="D55" t="s">
         <v>12</v>
@@ -3240,10 +3229,10 @@
         <v>106</v>
       </c>
       <c r="H55" t="s">
-        <v>239</v>
+        <v>232</v>
       </c>
       <c r="I55" t="s">
-        <v>251</v>
+        <v>244</v>
       </c>
       <c r="J55" t="s">
         <v>76</v>
@@ -3255,15 +3244,15 @@
         <v>-110.299927</v>
       </c>
     </row>
-    <row r="56" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A56">
         <v>55</v>
       </c>
       <c r="B56" t="s">
-        <v>170</v>
+        <v>166</v>
       </c>
       <c r="C56" t="s">
-        <v>171</v>
+        <v>167</v>
       </c>
       <c r="D56" t="s">
         <v>27</v>
@@ -3278,10 +3267,10 @@
         <v>239</v>
       </c>
       <c r="H56" t="s">
-        <v>238</v>
+        <v>231</v>
       </c>
       <c r="I56" t="s">
-        <v>250</v>
+        <v>243</v>
       </c>
       <c r="J56" t="s">
         <v>89</v>
@@ -3293,15 +3282,15 @@
         <v>-111.95251</v>
       </c>
     </row>
-    <row r="57" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A57">
         <v>56</v>
       </c>
       <c r="B57" t="s">
-        <v>172</v>
+        <v>168</v>
       </c>
       <c r="C57" t="s">
-        <v>173</v>
+        <v>169</v>
       </c>
       <c r="D57" t="s">
         <v>12</v>
@@ -3316,10 +3305,10 @@
         <v>100</v>
       </c>
       <c r="H57" t="s">
-        <v>244</v>
+        <v>237</v>
       </c>
       <c r="I57" t="s">
-        <v>248</v>
+        <v>241</v>
       </c>
       <c r="J57" t="s">
         <v>18</v>
@@ -3331,15 +3320,15 @@
         <v>-112.0269964</v>
       </c>
     </row>
-    <row r="58" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A58">
         <v>57</v>
       </c>
       <c r="B58" t="s">
-        <v>174</v>
+        <v>170</v>
       </c>
       <c r="C58" t="s">
-        <v>175</v>
+        <v>171</v>
       </c>
       <c r="D58" t="s">
         <v>12</v>
@@ -3354,13 +3343,13 @@
         <v>175</v>
       </c>
       <c r="H58" t="s">
-        <v>243</v>
+        <v>236</v>
       </c>
       <c r="I58" t="s">
-        <v>252</v>
+        <v>245</v>
       </c>
       <c r="J58" t="s">
-        <v>176</v>
+        <v>172</v>
       </c>
       <c r="K58">
         <v>33.621246678571417</v>
@@ -3369,15 +3358,15 @@
         <v>-112.1858287</v>
       </c>
     </row>
-    <row r="59" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A59">
         <v>58</v>
       </c>
       <c r="B59" t="s">
-        <v>177</v>
+        <v>173</v>
       </c>
       <c r="C59" t="s">
-        <v>178</v>
+        <v>174</v>
       </c>
       <c r="D59" t="s">
         <v>12</v>
@@ -3392,7 +3381,7 @@
         <v>130</v>
       </c>
       <c r="H59" t="s">
-        <v>238</v>
+        <v>231</v>
       </c>
       <c r="J59" t="s">
         <v>100</v>
@@ -3404,15 +3393,15 @@
         <v>-95.458209269999998</v>
       </c>
     </row>
-    <row r="60" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A60">
         <v>59</v>
       </c>
       <c r="B60" t="s">
-        <v>179</v>
+        <v>175</v>
       </c>
       <c r="C60" t="s">
-        <v>180</v>
+        <v>176</v>
       </c>
       <c r="D60" t="s">
         <v>43</v>
@@ -3427,13 +3416,13 @@
         <v>150</v>
       </c>
       <c r="H60" t="s">
-        <v>247</v>
+        <v>240</v>
       </c>
       <c r="I60" t="s">
-        <v>250</v>
+        <v>243</v>
       </c>
       <c r="J60" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="K60">
         <v>33.562936499999999</v>
@@ -3442,15 +3431,15 @@
         <v>-112.10580589999999</v>
       </c>
     </row>
-    <row r="61" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A61">
         <v>60</v>
       </c>
       <c r="B61" t="s">
-        <v>181</v>
+        <v>177</v>
       </c>
       <c r="C61" t="s">
-        <v>182</v>
+        <v>178</v>
       </c>
       <c r="D61" t="s">
         <v>43</v>
@@ -3465,13 +3454,13 @@
         <v>48</v>
       </c>
       <c r="H61" t="s">
-        <v>244</v>
+        <v>237</v>
       </c>
       <c r="I61" t="s">
-        <v>249</v>
+        <v>242</v>
       </c>
       <c r="J61" t="s">
-        <v>183</v>
+        <v>179</v>
       </c>
       <c r="K61">
         <v>33.4239453</v>
@@ -3480,15 +3469,15 @@
         <v>-111.838646</v>
       </c>
     </row>
-    <row r="62" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A62">
         <v>61</v>
       </c>
       <c r="B62" t="s">
-        <v>184</v>
+        <v>180</v>
       </c>
       <c r="C62" t="s">
-        <v>185</v>
+        <v>181</v>
       </c>
       <c r="D62" t="s">
         <v>43</v>
@@ -3503,13 +3492,13 @@
         <v>87</v>
       </c>
       <c r="H62" t="s">
-        <v>244</v>
+        <v>237</v>
       </c>
       <c r="I62" t="s">
-        <v>249</v>
+        <v>242</v>
       </c>
       <c r="J62" t="s">
-        <v>183</v>
+        <v>179</v>
       </c>
       <c r="K62">
         <v>33.429537921030061</v>
@@ -3518,15 +3507,15 @@
         <v>-111.8408907</v>
       </c>
     </row>
-    <row r="63" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A63">
         <v>62</v>
       </c>
       <c r="B63" t="s">
-        <v>186</v>
+        <v>182</v>
       </c>
       <c r="C63" t="s">
-        <v>187</v>
+        <v>183</v>
       </c>
       <c r="D63" t="s">
         <v>128</v>
@@ -3541,13 +3530,13 @@
         <v>304</v>
       </c>
       <c r="H63" t="s">
-        <v>240</v>
+        <v>233</v>
       </c>
       <c r="I63" t="s">
-        <v>252</v>
+        <v>245</v>
       </c>
       <c r="J63" t="s">
-        <v>188</v>
+        <v>184</v>
       </c>
       <c r="K63">
         <v>33.513083999999999</v>
@@ -3556,15 +3545,15 @@
         <v>-112.1795159</v>
       </c>
     </row>
-    <row r="64" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A64">
         <v>63</v>
       </c>
       <c r="B64" t="s">
-        <v>189</v>
+        <v>185</v>
       </c>
       <c r="C64" t="s">
-        <v>159</v>
+        <v>156</v>
       </c>
       <c r="D64" t="s">
         <v>12</v>
@@ -3579,13 +3568,13 @@
         <v>68</v>
       </c>
       <c r="H64" t="s">
-        <v>240</v>
+        <v>233</v>
       </c>
       <c r="I64" t="s">
-        <v>249</v>
+        <v>242</v>
       </c>
       <c r="J64" t="s">
-        <v>188</v>
+        <v>184</v>
       </c>
       <c r="K64">
         <v>33.499935000000001</v>
@@ -3594,15 +3583,15 @@
         <v>-112.10819979999999</v>
       </c>
     </row>
-    <row r="65" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A65">
         <v>64</v>
       </c>
       <c r="B65" t="s">
-        <v>190</v>
+        <v>186</v>
       </c>
       <c r="C65" t="s">
-        <v>191</v>
+        <v>187</v>
       </c>
       <c r="D65" t="s">
         <v>52</v>
@@ -3617,13 +3606,13 @@
         <v>84</v>
       </c>
       <c r="H65" t="s">
-        <v>242</v>
+        <v>235</v>
       </c>
       <c r="I65" t="s">
-        <v>251</v>
+        <v>244</v>
       </c>
       <c r="J65" t="s">
-        <v>192</v>
+        <v>188</v>
       </c>
       <c r="K65">
         <v>35.063642000000002</v>
@@ -3632,15 +3621,15 @@
         <v>-106.58319299999999</v>
       </c>
     </row>
-    <row r="66" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A66">
         <v>65</v>
       </c>
       <c r="B66" t="s">
-        <v>193</v>
+        <v>189</v>
       </c>
       <c r="C66" t="s">
-        <v>194</v>
+        <v>190</v>
       </c>
       <c r="D66" t="s">
         <v>27</v>
@@ -3655,13 +3644,13 @@
         <v>88</v>
       </c>
       <c r="H66" t="s">
-        <v>244</v>
+        <v>237</v>
       </c>
       <c r="I66" t="s">
-        <v>248</v>
+        <v>241</v>
       </c>
       <c r="J66" t="s">
-        <v>183</v>
+        <v>179</v>
       </c>
       <c r="K66">
         <v>33.392924802180318</v>
@@ -3670,15 +3659,15 @@
         <v>-111.9122897</v>
       </c>
     </row>
-    <row r="67" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A67">
         <v>66</v>
       </c>
       <c r="B67" t="s">
-        <v>195</v>
+        <v>191</v>
       </c>
       <c r="C67" t="s">
-        <v>196</v>
+        <v>192</v>
       </c>
       <c r="D67" t="s">
         <v>12</v>
@@ -3693,10 +3682,10 @@
         <v>15</v>
       </c>
       <c r="H67" t="s">
-        <v>240</v>
+        <v>233</v>
       </c>
       <c r="I67" t="s">
-        <v>249</v>
+        <v>242</v>
       </c>
       <c r="J67" t="s">
         <v>119</v>
@@ -3708,15 +3697,15 @@
         <v>-112.0653233</v>
       </c>
     </row>
-    <row r="68" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A68">
         <v>67</v>
       </c>
       <c r="B68" t="s">
-        <v>197</v>
+        <v>193</v>
       </c>
       <c r="C68" t="s">
-        <v>198</v>
+        <v>194</v>
       </c>
       <c r="D68" t="s">
         <v>12</v>
@@ -3731,10 +3720,10 @@
         <v>130</v>
       </c>
       <c r="H68" t="s">
-        <v>244</v>
+        <v>237</v>
       </c>
       <c r="I68" t="s">
-        <v>252</v>
+        <v>245</v>
       </c>
       <c r="J68" t="s">
         <v>72</v>
@@ -3746,15 +3735,15 @@
         <v>-112.0522514</v>
       </c>
     </row>
-    <row r="69" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A69">
         <v>68</v>
       </c>
       <c r="B69" t="s">
-        <v>199</v>
+        <v>195</v>
       </c>
       <c r="C69" t="s">
-        <v>200</v>
+        <v>196</v>
       </c>
       <c r="D69" t="s">
         <v>114</v>
@@ -3769,13 +3758,13 @@
         <v>51</v>
       </c>
       <c r="H69" t="s">
-        <v>242</v>
+        <v>235</v>
       </c>
       <c r="I69" t="s">
-        <v>251</v>
+        <v>244</v>
       </c>
       <c r="J69" t="s">
-        <v>201</v>
+        <v>197</v>
       </c>
       <c r="K69">
         <v>35.060535000000002</v>
@@ -3784,18 +3773,18 @@
         <v>-106.5819166</v>
       </c>
     </row>
-    <row r="70" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A70">
         <v>69</v>
       </c>
       <c r="B70" t="s">
-        <v>202</v>
+        <v>198</v>
       </c>
       <c r="C70" t="s">
-        <v>203</v>
+        <v>199</v>
       </c>
       <c r="D70" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="E70" t="s">
         <v>13</v>
@@ -3807,13 +3796,13 @@
         <v>100</v>
       </c>
       <c r="H70" t="s">
-        <v>244</v>
+        <v>237</v>
       </c>
       <c r="I70" t="s">
-        <v>248</v>
+        <v>241</v>
       </c>
       <c r="J70" t="s">
-        <v>183</v>
+        <v>179</v>
       </c>
       <c r="K70">
         <v>33.583382776327859</v>
@@ -3822,15 +3811,15 @@
         <v>-112.24212970000001</v>
       </c>
     </row>
-    <row r="71" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A71">
         <v>70</v>
       </c>
       <c r="B71" t="s">
-        <v>204</v>
+        <v>200</v>
       </c>
       <c r="C71" t="s">
-        <v>205</v>
+        <v>201</v>
       </c>
       <c r="D71" t="s">
         <v>114</v>
@@ -3845,13 +3834,13 @@
         <v>157</v>
       </c>
       <c r="H71" t="s">
-        <v>242</v>
+        <v>235</v>
       </c>
       <c r="I71" t="s">
-        <v>251</v>
+        <v>244</v>
       </c>
       <c r="J71" t="s">
-        <v>192</v>
+        <v>188</v>
       </c>
       <c r="K71">
         <v>35.130417850000001</v>
@@ -3860,15 +3849,15 @@
         <v>-106.5809929</v>
       </c>
     </row>
-    <row r="72" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A72">
         <v>71</v>
       </c>
       <c r="B72" t="s">
-        <v>206</v>
+        <v>202</v>
       </c>
       <c r="C72" t="s">
-        <v>207</v>
+        <v>203</v>
       </c>
       <c r="D72" t="s">
         <v>12</v>
@@ -3883,13 +3872,13 @@
         <v>93</v>
       </c>
       <c r="H72" t="s">
-        <v>247</v>
+        <v>240</v>
       </c>
       <c r="I72" t="s">
-        <v>250</v>
+        <v>243</v>
       </c>
       <c r="J72" t="s">
-        <v>162</v>
+        <v>158</v>
       </c>
       <c r="K72">
         <v>33.507791929292928</v>
@@ -3898,15 +3887,15 @@
         <v>-112.0913487</v>
       </c>
     </row>
-    <row r="73" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A73">
         <v>72</v>
       </c>
       <c r="B73" t="s">
-        <v>208</v>
+        <v>204</v>
       </c>
       <c r="C73" t="s">
-        <v>209</v>
+        <v>205</v>
       </c>
       <c r="D73" t="s">
         <v>12</v>
@@ -3921,10 +3910,10 @@
         <v>219</v>
       </c>
       <c r="H73" t="s">
-        <v>238</v>
+        <v>231</v>
       </c>
       <c r="I73" t="s">
-        <v>250</v>
+        <v>243</v>
       </c>
       <c r="J73" t="s">
         <v>89</v>
@@ -3936,21 +3925,21 @@
         <v>-112.06497299999999</v>
       </c>
     </row>
-    <row r="74" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A74">
         <v>73</v>
       </c>
       <c r="B74" t="s">
-        <v>210</v>
+        <v>206</v>
       </c>
       <c r="C74" t="s">
-        <v>211</v>
+        <v>207</v>
       </c>
       <c r="D74" t="s">
-        <v>212</v>
+        <v>208</v>
       </c>
       <c r="E74" t="s">
-        <v>213</v>
+        <v>209</v>
       </c>
       <c r="F74">
         <v>89113</v>
@@ -3959,10 +3948,10 @@
         <v>308</v>
       </c>
       <c r="H74" t="s">
-        <v>241</v>
+        <v>234</v>
       </c>
       <c r="I74" t="s">
-        <v>251</v>
+        <v>244</v>
       </c>
       <c r="J74" t="s">
         <v>21</v>
@@ -3974,18 +3963,18 @@
         <v>-115.2608364</v>
       </c>
     </row>
-    <row r="75" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A75">
         <v>74</v>
       </c>
       <c r="B75" t="s">
-        <v>214</v>
+        <v>210</v>
       </c>
       <c r="C75" t="s">
-        <v>215</v>
+        <v>211</v>
       </c>
       <c r="D75" t="s">
-        <v>167</v>
+        <v>163</v>
       </c>
       <c r="E75" t="s">
         <v>99</v>
@@ -3997,7 +3986,7 @@
         <v>120</v>
       </c>
       <c r="H75" t="s">
-        <v>238</v>
+        <v>231</v>
       </c>
       <c r="J75" t="s">
         <v>100</v>
@@ -4009,15 +3998,15 @@
         <v>-95.556236080000005</v>
       </c>
     </row>
-    <row r="76" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A76">
         <v>75</v>
       </c>
       <c r="B76" t="s">
-        <v>216</v>
+        <v>212</v>
       </c>
       <c r="C76" t="s">
-        <v>217</v>
+        <v>213</v>
       </c>
       <c r="D76" t="s">
         <v>27</v>
@@ -4032,13 +4021,13 @@
         <v>90</v>
       </c>
       <c r="H76" t="s">
-        <v>240</v>
+        <v>233</v>
       </c>
       <c r="I76" t="s">
-        <v>252</v>
+        <v>245</v>
       </c>
       <c r="J76" t="s">
-        <v>218</v>
+        <v>214</v>
       </c>
       <c r="K76">
         <v>33.422002080715657</v>
@@ -4047,53 +4036,20 @@
         <v>-111.8948358</v>
       </c>
     </row>
-    <row r="77" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A77">
         <v>77</v>
       </c>
-      <c r="B77" t="s">
-        <v>219</v>
-      </c>
-      <c r="C77" t="s">
-        <v>220</v>
-      </c>
-      <c r="D77" t="s">
-        <v>12</v>
-      </c>
-      <c r="E77" t="s">
-        <v>13</v>
-      </c>
-      <c r="F77">
-        <v>85021</v>
-      </c>
-      <c r="G77">
-        <v>148</v>
-      </c>
-      <c r="H77" t="s">
-        <v>238</v>
-      </c>
-      <c r="I77" t="s">
-        <v>250</v>
-      </c>
-      <c r="J77" t="s">
-        <v>221</v>
-      </c>
-      <c r="K77">
-        <v>33.538449423728807</v>
-      </c>
-      <c r="L77">
-        <v>-112.0930852</v>
-      </c>
-    </row>
-    <row r="78" spans="1:12" x14ac:dyDescent="0.25">
+    </row>
+    <row r="78" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A78">
         <v>78</v>
       </c>
       <c r="B78" t="s">
-        <v>222</v>
+        <v>215</v>
       </c>
       <c r="C78" t="s">
-        <v>223</v>
+        <v>216</v>
       </c>
       <c r="D78" t="s">
         <v>12</v>
@@ -4108,10 +4064,10 @@
         <v>36</v>
       </c>
       <c r="H78" t="s">
-        <v>245</v>
+        <v>238</v>
       </c>
       <c r="I78" t="s">
-        <v>250</v>
+        <v>243</v>
       </c>
       <c r="J78" t="s">
         <v>95</v>
@@ -4123,15 +4079,15 @@
         <v>-112.08100349999999</v>
       </c>
     </row>
-    <row r="79" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A79">
         <v>79</v>
       </c>
       <c r="B79" t="s">
-        <v>224</v>
+        <v>217</v>
       </c>
       <c r="C79" t="s">
-        <v>225</v>
+        <v>218</v>
       </c>
       <c r="D79" t="s">
         <v>86</v>
@@ -4146,10 +4102,10 @@
         <v>80</v>
       </c>
       <c r="H79" t="s">
-        <v>243</v>
+        <v>236</v>
       </c>
       <c r="I79" t="s">
-        <v>248</v>
+        <v>241</v>
       </c>
       <c r="J79" t="s">
         <v>21</v>
@@ -4161,15 +4117,15 @@
         <v>-111.7900037</v>
       </c>
     </row>
-    <row r="80" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A80">
         <v>80</v>
       </c>
       <c r="B80" t="s">
-        <v>226</v>
+        <v>219</v>
       </c>
       <c r="C80" t="s">
-        <v>227</v>
+        <v>220</v>
       </c>
       <c r="D80" t="s">
         <v>12</v>
@@ -4184,13 +4140,13 @@
         <v>104</v>
       </c>
       <c r="H80" t="s">
-        <v>240</v>
+        <v>233</v>
       </c>
       <c r="I80" t="s">
-        <v>249</v>
+        <v>242</v>
       </c>
       <c r="J80" t="s">
-        <v>218</v>
+        <v>214</v>
       </c>
       <c r="K80">
         <v>33.530325300000001</v>
@@ -4199,15 +4155,15 @@
         <v>-112.0559015</v>
       </c>
     </row>
-    <row r="81" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A81">
         <v>81</v>
       </c>
       <c r="B81" t="s">
-        <v>228</v>
+        <v>221</v>
       </c>
       <c r="C81" t="s">
-        <v>229</v>
+        <v>222</v>
       </c>
       <c r="D81" t="s">
         <v>65</v>
@@ -4222,13 +4178,13 @@
         <v>205</v>
       </c>
       <c r="H81" t="s">
-        <v>239</v>
+        <v>232</v>
       </c>
       <c r="I81" t="s">
-        <v>251</v>
+        <v>244</v>
       </c>
       <c r="J81" t="s">
-        <v>230</v>
+        <v>223</v>
       </c>
       <c r="K81">
         <v>32.236018818181819</v>
@@ -4237,15 +4193,15 @@
         <v>-111.0150285</v>
       </c>
     </row>
-    <row r="82" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A82">
         <v>82</v>
       </c>
       <c r="B82" t="s">
-        <v>231</v>
+        <v>224</v>
       </c>
       <c r="C82" t="s">
-        <v>232</v>
+        <v>225</v>
       </c>
       <c r="D82" t="s">
         <v>12</v>
@@ -4260,10 +4216,10 @@
         <v>99</v>
       </c>
       <c r="H82" t="s">
-        <v>247</v>
+        <v>240</v>
       </c>
       <c r="I82" t="s">
-        <v>250</v>
+        <v>243</v>
       </c>
       <c r="J82" t="s">
         <v>122</v>
@@ -4275,15 +4231,15 @@
         <v>-112.097089</v>
       </c>
     </row>
-    <row r="83" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A83">
         <v>83</v>
       </c>
       <c r="B83" t="s">
-        <v>233</v>
+        <v>226</v>
       </c>
       <c r="C83" t="s">
-        <v>234</v>
+        <v>227</v>
       </c>
       <c r="D83" t="s">
         <v>86</v>
@@ -4298,10 +4254,10 @@
         <v>76</v>
       </c>
       <c r="H83" t="s">
+        <v>236</v>
+      </c>
+      <c r="I83" t="s">
         <v>243</v>
-      </c>
-      <c r="I83" t="s">
-        <v>250</v>
       </c>
       <c r="J83" t="s">
         <v>17</v>

</xml_diff>